<commit_message>
Bug fixes with array sizes
</commit_message>
<xml_diff>
--- a/Jeannine's log.xlsx
+++ b/Jeannine's log.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan\Documents\Visual Studio 2015\Projects\ClassOpsLogCreator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="90" yWindow="150" windowWidth="14865" windowHeight="10785" tabRatio="440"/>
   </bookViews>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="109">
   <si>
     <t>Staff Name</t>
   </si>
@@ -354,7 +359,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -531,6 +536,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -578,7 +586,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -611,9 +619,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -646,6 +671,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -825,10 +867,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="A3:F5"/>
+      <selection activeCell="A5" sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,6 +921,86 @@
         <v>107</v>
       </c>
       <c r="F2" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="10">
+        <v>42570</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="10">
+        <v>42570</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="10">
+        <v>42570</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="10">
+        <v>42570</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed a bug where there is no entry for the day
</commit_message>
<xml_diff>
--- a/Jeannine's log.xlsx
+++ b/Jeannine's log.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="109">
   <si>
     <t>Staff Name</t>
   </si>
@@ -867,10 +867,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,7 +909,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="10">
-        <v>42571</v>
+        <v>42570</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>106</v>
@@ -921,86 +921,6 @@
         <v>107</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="10">
-        <v>42571</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="10">
-        <v>42571</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="10">
-        <v>42571</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="10">
-        <v>42571</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F6" s="19" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>